<commit_message>
Edit Sheet ke 3
</commit_message>
<xml_diff>
--- a/Ringkasan Saham-minggu ke2 Juni 2020.xlsx
+++ b/Ringkasan Saham-minggu ke2 Juni 2020.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="15 Juni" sheetId="1" r:id="rId1"/>
     <sheet name="16 Juni" sheetId="2" r:id="rId2"/>
-    <sheet name="17 Juni" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'15 Juni'!$A$1:$AB$697</definedName>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4215" uniqueCount="1416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4219" uniqueCount="1420">
   <si>
     <t>No</t>
   </si>
@@ -4269,6 +4269,18 @@
   </si>
   <si>
     <t>Net Foreign BUY/SELL</t>
+  </si>
+  <si>
+    <t>qewfgasdfzxcvbdfg</t>
+  </si>
+  <si>
+    <t>sfe</t>
+  </si>
+  <si>
+    <t>asdfsdf</t>
+  </si>
+  <si>
+    <t>sadf</t>
   </si>
 </sst>
 </file>
@@ -102846,12 +102858,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="C6" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="D8" t="s">
+        <v>1418</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>